<commit_message>
initial script data cleaning and sentiment analysis
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\UCI Data Science\Projects\UCI-Project-3\myFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{317319C8-5C67-41E9-8A79-6F1DEA9576D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0DC6B833-509B-46B5-BB8E-F99EE6265E77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6620" xr2:uid="{156198FB-929A-49EB-8FA5-1B48AF623262}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -284,6 +284,33 @@
   </si>
   <si>
     <t>CG</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>get a reviews data set for sentiment analysis</t>
+  </si>
+  <si>
+    <t>reload original CSV, and do a count of unique characters per episode</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>count # of rows per episode</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>VADER Sentiment</t>
+  </si>
+  <si>
+    <t>add a new column -- if MainChar then == Sentiment else NaN</t>
+  </si>
+  <si>
+    <t>same as above but specific to each MainChar</t>
   </si>
 </sst>
 </file>
@@ -348,13 +375,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="9"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,7 +400,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -494,246 +525,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1047,13 +838,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35871B35-CB0B-4972-85AE-8FE5A9F65723}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1063,34 +854,34 @@
     <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1102,19 +893,19 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>43200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" s="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
@@ -1126,38 +917,43 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>43200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A4" s="3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="2">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A5" s="3">
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="2">
         <f t="shared" ref="A5:A11" si="0">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
@@ -1169,14 +965,20 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A6" s="3">
+      <c r="F5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
@@ -1188,14 +990,18 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A7" s="3">
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="s">
@@ -1207,14 +1013,22 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A8" s="3">
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43202</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
@@ -1226,14 +1040,18 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A9" s="3">
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
@@ -1245,14 +1063,18 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A10" s="3">
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
@@ -1264,17 +1086,18 @@
       <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A11" s="3">
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
@@ -1283,27 +1106,36 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C12" s="1"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C13" s="1"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="C14" s="2"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C15" s="1"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C16" s="1"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C17" s="1"/>
@@ -1313,33 +1145,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F12:F16">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Question Pending">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Question Pending">
       <formula>NOT(ISERROR(SEARCH("Question Pending",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Question">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Question">
       <formula>NOT(ISERROR(SEARCH("Question",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="On Hold">
+      <formula>NOT(ISERROR(SEARCH("On Hold",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:F16" xr:uid="{F7A04D5B-C7B4-4C96-AD88-3D1A98978BF9}">
       <formula1>"Not Started, In Progress, Question Pending, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{E2C27111-C09B-4642-AFBF-4BB5CD113A97}">
-      <formula1>"Question Pending, In Progress, Complete"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11" xr:uid="{4578FAC2-A386-4693-838B-7973DF8B6E44}">
+      <formula1>"Question Pending, In Progress, Complete, On Hold"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>